<commit_message>
Finished support for multiple plate in CFrenaming
</commit_message>
<xml_diff>
--- a/demoSamples/renamingCF2.xlsx
+++ b/demoSamples/renamingCF2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiton\Documents\PyCodes\EasyFlowQ\demoSamples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yma2\Documents\PythonCodes\EasyFlowQ\demoSamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9519A3-45CE-48AA-8356-ABBAC4925505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A376D6-FAA8-419E-9391-0EAB02BE0372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="290" windowWidth="18390" windowHeight="11710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>smpl1</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>uniquex3</t>
+  </si>
+  <si>
+    <t>plate2</t>
+  </si>
+  <si>
+    <t>Plate2P1</t>
   </si>
 </sst>
 </file>
@@ -377,37 +383,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -424,44 +435,44 @@
       <selection activeCell="B8" sqref="B8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -473,52 +484,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA705DE4-3873-444E-9B82-5FD8C2247234}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>